<commit_message>
fun_test with para ok
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="89">
   <si>
     <t>data1</t>
   </si>
@@ -249,6 +249,108 @@
   </si>
   <si>
     <t>L10 = list(L1 = NULL, L2 = c(0, 45, 90, 180, 270, 361, -90), L3 = list(data.frame()))</t>
+  </si>
+  <si>
+    <t>Ok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+set.seed(1) ; obs1 &lt;- data.frame(Time = c(rnorm(10), rnorm(10) + 2), Group1 = rep(c("G", "H"), each = 10)) ; 
+a &lt;- fun_test(
+arg = c("data1", "y", "categ"),
+val = list(
+L1 = list(L1 = NULL, L2 = obs1, L3 = "a"), 
+L2 = list(L1 = NULL, L2 = "Time", L3 = list(data.frame())), 
+L3 = list(L1 = NULL, L2 = "Group1", L3 = c("Group1", "Group2"), L4 = list(data.frame()))
+),
+thread.nb = 7,
+fun = "fun_gg_boxplot",
+plot.fun = TRUE,
+res.path = "C:\\Users\\Gael\\Desktop\\"
+)
+</t>
+  </si>
+  <si>
+    <t>L2 = list(L1 ="Time")</t>
+  </si>
+  <si>
+    <t>L3 = list(L1 = "Group1")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+set.seed(1) ; obs1 &lt;- data.frame(Time = c(rnorm(10), rnorm(10) + 2), Group1 = rep(c("G", "H"), each = 10)) ; 
+a &lt;- fun_test(
+arg = c("data1", "y", "categ", "categ.class.order", "categ.legend.name", "categ.color"),
+val = list(
+L1 = list(L1 = obs1),
+L2 = list(L1 ="Time"),
+L3 = list(L1 = "Group1"),
+L4 = list(L1 = NULL, L2 = list(c("G", "H")), L2 = list(c("H", "G")), L2 = list(c("G", "H"), c("A", "B")), L3 = list(c("H", "G"), c("A", "B")), L4 = list(c("H", "G"), c("B", "A")), L5 = list(data.frame())),
+L5 = list(L1 = NULL, L2 = "CLASS1", L3 = list(data.frame())),
+L6 = list(L1 = NULL, L2 = "green", L3 = c("blue", "green"), L4 = c("green", "blue"), L5 = list(data.frame()))
+),
+thread.nb = NULL,
+fun = "fun_gg_boxplot",
+plot.fun = TRUE,
+res.path = "C:\\Users\\Gael\\Desktop\\",
+export = TRUE
+)
+</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">set.seed(1) ; obs1 &lt;- data.frame(Time = c(rnorm(20), rnorm(20) + 2), Group1 = rep(c("G", "H"), each = 10), Group2 = rep(c("A", "B"), time = 10)) ; 
+a &lt;- fun_test(
+arg = c("data1", "y", "categ", "categ.class.order", "categ.legend.name", "categ.color", "box.fill", "box.width", "box.space", "box.line.size", "box.notch", "box.alpha", "box.mean", "box.whisker.kind", "box.whisker.width", "dot.color", "dot.categ", "dot.categ.class.order", "dot.categ.legend.name", "dot.tidy", "dot.tidy.bin.nb", "dot.jitter", "dot.size", "dot.alpha", "dot.border.size", "dot.border.color"),
+val = list(
+l = list(
+L1 = list(L1 =  obs1), 
+L2 = list(L1 = "Time"), 
+L3 = list(L1 = "Group1", L3 = c("Group1", "Group2")), 
+L4 = list(L2 = list(c("G", "H")), L2 = list(c("H", "G")), L2 = list(c("G", "H"), c("A", "B")), L3 = list(c("H", "G"), c("A", "B")), L4 = list(c("H", "G"), c("B", "A"))),
+L6 = list(L2 = "green", L3 = c("blue", "green"), L4 = c("green", "blue")), 
+L7 = list(L1 = NULL, L2 = c(TRUE, FALSE), L3 = list(data.frame())), 
+L8 = list(L1 = NULL, L2 = c(0, 0.5, 1), L3 = list(data.frame())), 
+L8 = list(L1 = NULL, L2 = c(0, 0.5, 1), L3 = list(data.frame())), 
+L8 = list(L1 = NULL, L2 = c(0, 0.5, 1), L3 = list(data.frame())), 
+L7 = list(L1 = NULL, L2 = c(TRUE, FALSE), L3 = list(data.frame())), 
+L8 = list(L1 = NULL, L2 = c(0, 0.5, 1), L3 = list(data.frame())), 
+L7 = list(L1 = NULL, L2 = c(TRUE, FALSE), L3 = list(data.frame())), 
+L7 = list(L1 = NULL, L2 = c("no", "std", "max"), L3 = list(data.frame())), 
+L8 = list(L1 = NULL, L2 = c(0, 0.5, 1), L3 = list(data.frame())), 
+L6 = list(L1 = NULL, L2 = "black", L3 = "same", L4 = c("green", "blue"), L3 = list(data.frame())), 
+L6 = list(L1 = NULL, L2 = c("Group2", "TEST_ERROR"), L3 = list(data.frame())), 
+L6 = list(L1 = NULL, L2 = "Group2", L3 = c("B", "A"), L3 = list(data.frame())), 
+L5 = list(L1 = NULL, L2 = "DOT1", L3 = list(data.frame())), 
+L7 = list(L1 = NULL, L2 = c(TRUE, FALSE), L3 = list(data.frame())), 
+L8 = list(L1 = NULL, L2 = c(0, 30, 50, -1), L3 = list(data.frame())), 
+L8 = list(L1 = NULL, L2 = c(0, 0.5, 1), L3 = list(data.frame())), 
+L8 = list(L1 = NULL, L2 = c(0, 0.5, 1), L3 = list(data.frame())), 
+L8 = list(L1 = NULL, L2 = c(0, 0.5, 1), L3 = list(data.frame())), 
+L8 = list(L1 = NULL, L2 = c(0, 0.5, 1), L3 = list(data.frame())), 
+L10 = list(L1 = NULL, L2 = "blue", L3 = 2, L3 = list(data.frame()))
+),
+thread.nb = 7,
+fun = "fun_gg_boxplot",
+plot.fun = TRUE,
+res.path = "C:\\Users\\Gael\\Desktop\\",
+export = TRUE
+)
+</t>
+  </si>
+  <si>
+    <t>L1 = list(L1 =obs1)</t>
+  </si>
+  <si>
+    <t>L3 = list(L1 = "Group1", L3 = c("Group1", "Group2"))</t>
+  </si>
+  <si>
+    <t>L4 = list(L2 = list(c("G", "H")), L2 = list(c("H", "G")), L2 = list(c("G", "H"), c("A", "B")), L3 = list(c("H", "G"), c("A", "B")), L4 = list(c("H", "G"), c("B", "A")))</t>
+  </si>
+  <si>
+    <t>L6 = list(L2 = "green", L3 = c("blue", "green"), L4 = c("green", "blue"))</t>
   </si>
 </sst>
 </file>
@@ -291,9 +393,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -595,428 +705,525 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="58.109375" customWidth="1"/>
+    <col min="1" max="1" width="25" style="1" customWidth="1"/>
+    <col min="2" max="2" width="161" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" ht="219" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="6" spans="1:9" ht="288" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B10" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B11" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B12" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="17" spans="1:2" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B24" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B25" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B26" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B27" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B28" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B29" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B30" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B31" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B32" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B33" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B34" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B35" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B36" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B37" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B38" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B39" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B40" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B41" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B42" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B43" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B65" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B66" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B67" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B68" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B69" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B70" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B71" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B72" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B73" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B74" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B75" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B76" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B77" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B78" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B79" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B80" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B81" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B82" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B83" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B84" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B85" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B86" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B87" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B88" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B89" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B52" s="1"/>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B90" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fun_test and boxplot updated
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="110">
   <si>
     <t>data1</t>
   </si>
@@ -429,6 +429,29 @@
   </si>
   <si>
     <t xml:space="preserve">"categ.legend.name", </t>
+  </si>
+  <si>
+    <t xml:space="preserve">set.seed(1) ; obs1 &lt;- data.frame(Time = c(rnorm(20), rnorm(20) + 2), Group1 = rep(c("G", "H"), each = 10), Group2 = rep(c("A", "B"), time = 10)) ; 
+a &lt;- fun_test(
+arg = c("data1", "y", "categ", "categ.class.order", "categ.color", "dot.color", "dot.categ", "dot.categ.class.order", "dot.categ.legend.name"),
+val = list(
+L1 = list(L1 =  obs1), 
+L2 = list(L1 = "Time"), 
+L3 = list(L1 = "Group1", L3 = c("Group1", "Group2")), 
+L4 = list(L2 = list(c("G", "H")), L2 = list(c("H", "G")), L2 = list(c("G", "H"), c("A", "B")), L3 = list(c("H", "G"), c("A", "B")), L4 = list(c("H", "G"), c("B", "A"))),
+L6 = list(L1 = NULL, L2 = "green", L3 = c("blue", "green"), L4 = c("green", "blue")), 
+L7 = list(L1 = "same", L2 = NULL, L3= "black", L4 = c("red", "brown")), 
+L6 = list(L2 = c("Group1")), 
+L6 = list(L1 = NULL, L2 = c("G", "H"), L2 = c("H", "G")), 
+L5 = list(L2 = NULL, L2 = "DOT1")
+),
+thread.nb = 7,
+fun = "fun_gg_boxplot",
+plot.fun = TRUE,
+res.path = "C:\\Users\\Gael\\Desktop\\",
+export = TRUE
+)
+</t>
   </si>
 </sst>
 </file>
@@ -792,10 +815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I108"/>
+  <dimension ref="A1:I118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -983,194 +1006,194 @@
       <c r="B28" s="2"/>
     </row>
     <row r="29" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="2"/>
+      <c r="A29" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="30" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="2"/>
+      <c r="A30" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="31" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="2"/>
+      <c r="A31" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="32" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="2"/>
+      <c r="A32" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="33" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="2"/>
+      <c r="A33" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="34" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="2"/>
+      <c r="A34" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="35" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="2"/>
+      <c r="A35" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="36" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>82</v>
+      <c r="A36" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>78</v>
+      <c r="A37" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>83</v>
+      <c r="A38" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>84</v>
-      </c>
+      <c r="B39" s="2"/>
     </row>
     <row r="40" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="B40" s="2"/>
     </row>
     <row r="41" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>85</v>
-      </c>
+      <c r="B41" s="2"/>
     </row>
     <row r="42" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="B42" s="2"/>
     </row>
     <row r="43" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>57</v>
-      </c>
+      <c r="B43" s="2"/>
     </row>
     <row r="44" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>57</v>
-      </c>
+      <c r="B44" s="2"/>
     </row>
     <row r="45" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>57</v>
-      </c>
+      <c r="B45" s="2"/>
     </row>
     <row r="46" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>57</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>57</v>
@@ -1178,23 +1201,23 @@
     </row>
     <row r="58" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>57</v>
@@ -1202,175 +1225,175 @@
     </row>
     <row r="61" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B71" s="1" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>56</v>
@@ -1378,23 +1401,23 @@
     </row>
     <row r="104" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>56</v>
@@ -1402,14 +1425,94 @@
     </row>
     <row r="107" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="B117" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B108" s="3"/>
+    <row r="118" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B118" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fun_gg_boxplot now can display legend for dots with same column as boxplot
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -817,8 +817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19.2" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
lots of stuff fixed
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -817,8 +817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19.2" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>